<commit_message>
changes on price list
</commit_message>
<xml_diff>
--- a/Price List/Roboter Arm Price List.xlsx
+++ b/Price List/Roboter Arm Price List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TH24\Desktop\Hardware\Robotic-Arm\Price List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254BECC8-3750-4226-A98E-9AC0A8EE34E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D11B479-555D-45FA-943E-4F1CB1EA567F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24945" yWindow="0" windowWidth="23190" windowHeight="14535" xr2:uid="{6B6AC393-9DA6-4B7B-AC95-3B83A5A5BB6E}"/>
+    <workbookView xWindow="10515" yWindow="870" windowWidth="26025" windowHeight="14535" xr2:uid="{6B6AC393-9DA6-4B7B-AC95-3B83A5A5BB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Roboter Arm Main Controller" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Description</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>Gesamtpreis (Selbst bezahlt)</t>
+  </si>
+  <si>
+    <t>Custom Designed Controller with ESP32, ATMEAG USB-C Interface</t>
+  </si>
+  <si>
+    <t>Custom Designed Stepper Motor Controller on A4988 IC Nema 17</t>
+  </si>
+  <si>
+    <t>Custom Designed Stepper Motor Controller on A4988 IC Nema 11</t>
   </si>
 </sst>
 </file>
@@ -640,16 +649,16 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>
@@ -667,7 +676,7 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -678,7 +687,8 @@
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -692,7 +702,8 @@
         <f>23.99*2</f>
         <v>47.98</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -701,7 +712,8 @@
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -709,7 +721,8 @@
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,7 +732,8 @@
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -736,7 +750,8 @@
         <f>53.99*C7</f>
         <v>107.98</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="7"/>
@@ -755,7 +770,8 @@
         <f>31.94*C8</f>
         <v>95.820000000000007</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="7"/>
@@ -773,7 +789,8 @@
       <c r="D9" s="6">
         <v>14.85</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="7"/>
@@ -783,7 +800,8 @@
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="10"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,7 +809,8 @@
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -801,21 +820,25 @@
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="6">
         <v>47.4</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="10" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="7"/>
@@ -824,7 +847,9 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
@@ -832,7 +857,8 @@
         <f>24.834*C14</f>
         <v>49.667999999999999</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="10" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="7"/>
@@ -841,7 +867,9 @@
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C15" s="1">
         <v>3</v>
       </c>
@@ -849,7 +877,8 @@
         <f>19.35*C15</f>
         <v>58.050000000000004</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="10" t="s">
         <v>31</v>
       </c>
       <c r="H15" s="7"/>
@@ -859,14 +888,16 @@
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -876,7 +907,8 @@
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -892,7 +924,8 @@
       <c r="D19" s="6">
         <v>9.9600000000000009</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="10" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="7"/>
@@ -908,7 +941,8 @@
       <c r="D20" s="6">
         <v>6.99</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="10" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="7"/>
@@ -924,7 +958,8 @@
       <c r="D21" s="6">
         <v>26.21</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="10" t="s">
         <v>28</v>
       </c>
       <c r="H21" s="7"/>
@@ -940,7 +975,8 @@
       <c r="D22" s="6">
         <v>9.56</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="10" t="s">
         <v>32</v>
       </c>
       <c r="H22" s="7"/>
@@ -957,7 +993,8 @@
       <c r="D23" s="6">
         <v>2.4</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="10" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="7"/>
@@ -965,10 +1002,11 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H24" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="C26" s="12" t="s">
+    <row r="26" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B26" s="12" t="s">
         <v>40</v>
       </c>
+      <c r="C26" s="8"/>
       <c r="D26" s="8">
         <f>SUM(D2:D23)</f>
         <v>476.86799999999999</v>
@@ -978,10 +1016,11 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="C27" s="12" t="s">
+    <row r="27" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B27" s="12" t="s">
         <v>41</v>
       </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="8">
         <f>SUM(D21,D3)</f>
         <v>74.19</v>
@@ -990,10 +1029,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="C28" s="12" t="s">
+    <row r="28" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B28" s="12" t="s">
         <v>39</v>
       </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="8">
         <f>SUM(D2:D23)-D27</f>
         <v>402.678</v>
@@ -1004,20 +1044,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{080F4E5C-CE74-432E-843B-4C51967D58B5}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{B8D5915B-62D9-40A8-ACAA-9D669C08B368}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{CFB41B74-8990-4C22-A00D-6502C1D57934}"/>
-    <hyperlink ref="E14" r:id="rId4" xr:uid="{D9FDDAC3-87C6-4984-969F-4DF8CA76947C}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{AD4FC075-36B8-44E3-9A83-D09DD90BBCDD}"/>
-    <hyperlink ref="E13" r:id="rId6" xr:uid="{5693EB4A-F45D-41D3-9FFD-8F8E0EB0FF9F}"/>
-    <hyperlink ref="E19" r:id="rId7" display="https://www.amazon.de/-/en/Dadabig-Printer-Timing-Pulley-Pieces/dp/B07XHRQ8H1/ref=pd_sbs_2/257-1968653-5410067?pd_rd_w=5N9sg&amp;pf_rd_p=dd7cdb0d-7d18-43ba-a06d-a9f4cc6bae51&amp;pf_rd_r=PGHX3GXP813C0EZ4F4VJ&amp;pd_rd_r=a04a5175-06a3-4917-8c1d-eb5cf23b5fcd&amp;pd_rd_wg=LmMwN&amp;pd_rd_i=B07XHRQ8H1&amp;psc=1" xr:uid="{2926C0DD-673C-483C-81C1-1081A09FD741}"/>
-    <hyperlink ref="E20" r:id="rId8" display="https://www.amazon.de/-/en/sourcing-Round-Diameter-Length-Turning/dp/B07LBM311H/ref=pd_sbs_4/257-1968653-5410067?pd_rd_w=10MEQ&amp;pf_rd_p=dd7cdb0d-7d18-43ba-a06d-a9f4cc6bae51&amp;pf_rd_r=3E6030HAKWGWQ38FTRD2&amp;pd_rd_r=a0997397-9b9c-4197-8639-012eb4abc48f&amp;pd_rd_wg=ABNiX&amp;pd_rd_i=B07LBM311H&amp;psc=1" xr:uid="{BFF6BD90-2256-46AD-AF04-F740DC5A3FC8}"/>
-    <hyperlink ref="E21" r:id="rId9" xr:uid="{0AE23DBD-2E40-4019-A263-B0EE7AFC3C21}"/>
-    <hyperlink ref="E23" r:id="rId10" xr:uid="{CF4C82E1-5717-4D2D-A90E-848DBE0DC2AE}"/>
-    <hyperlink ref="E22" r:id="rId11" xr:uid="{AEB63538-6D56-42FD-9F2F-4B05E7217A61}"/>
-    <hyperlink ref="E3" r:id="rId12" xr:uid="{5CED3CA7-D874-4C19-AB98-4F24007D2E7D}"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{080F4E5C-CE74-432E-843B-4C51967D58B5}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{B8D5915B-62D9-40A8-ACAA-9D669C08B368}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{CFB41B74-8990-4C22-A00D-6502C1D57934}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{D9FDDAC3-87C6-4984-969F-4DF8CA76947C}"/>
+    <hyperlink ref="F15" r:id="rId5" xr:uid="{AD4FC075-36B8-44E3-9A83-D09DD90BBCDD}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{5693EB4A-F45D-41D3-9FFD-8F8E0EB0FF9F}"/>
+    <hyperlink ref="F19" r:id="rId7" display="https://www.amazon.de/-/en/Dadabig-Printer-Timing-Pulley-Pieces/dp/B07XHRQ8H1/ref=pd_sbs_2/257-1968653-5410067?pd_rd_w=5N9sg&amp;pf_rd_p=dd7cdb0d-7d18-43ba-a06d-a9f4cc6bae51&amp;pf_rd_r=PGHX3GXP813C0EZ4F4VJ&amp;pd_rd_r=a04a5175-06a3-4917-8c1d-eb5cf23b5fcd&amp;pd_rd_wg=LmMwN&amp;pd_rd_i=B07XHRQ8H1&amp;psc=1" xr:uid="{2926C0DD-673C-483C-81C1-1081A09FD741}"/>
+    <hyperlink ref="F20" r:id="rId8" display="https://www.amazon.de/-/en/sourcing-Round-Diameter-Length-Turning/dp/B07LBM311H/ref=pd_sbs_4/257-1968653-5410067?pd_rd_w=10MEQ&amp;pf_rd_p=dd7cdb0d-7d18-43ba-a06d-a9f4cc6bae51&amp;pf_rd_r=3E6030HAKWGWQ38FTRD2&amp;pd_rd_r=a0997397-9b9c-4197-8639-012eb4abc48f&amp;pd_rd_wg=ABNiX&amp;pd_rd_i=B07LBM311H&amp;psc=1" xr:uid="{BFF6BD90-2256-46AD-AF04-F740DC5A3FC8}"/>
+    <hyperlink ref="F21" r:id="rId9" xr:uid="{0AE23DBD-2E40-4019-A263-B0EE7AFC3C21}"/>
+    <hyperlink ref="F23" r:id="rId10" xr:uid="{CF4C82E1-5717-4D2D-A90E-848DBE0DC2AE}"/>
+    <hyperlink ref="F22" r:id="rId11" xr:uid="{AEB63538-6D56-42FD-9F2F-4B05E7217A61}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{5CED3CA7-D874-4C19-AB98-4F24007D2E7D}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>